<commit_message>
feat: add more diffs, refactor, plots
</commit_message>
<xml_diff>
--- a/res/SSBU25_dataset_samuel.xlsx
+++ b/res/SSBU25_dataset_samuel.xlsx
@@ -475,25 +475,25 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>diagnoza mkch-10</t>
+          <t>diagnoza MKCH-10</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>hfe c187g (h63d)
-[hfe]</t>
+          <t>HFE C187G (H63D)
+[HFE]</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>hfe a193t (s65c)
-[hfe]</t>
+          <t>HFE A193T (S65C)
+[HFE]</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>hfe g845a (c282y)
-[hfe]</t>
+          <t>HFE G845A (C282Y)
+[HFE]</t>
         </is>
       </c>
     </row>

</xml_diff>